<commit_message>
Updated the spring sheet
</commit_message>
<xml_diff>
--- a/sprintplanning_Online Movie.xlsx
+++ b/sprintplanning_Online Movie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\boot_capg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E677D9B4-AA1F-4585-AC34-07B241B6F9B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D087697B-759E-4789-8255-5C666B874698}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User stories" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="85">
   <si>
     <t>Main User Story</t>
   </si>
@@ -175,36 +175,9 @@
     <t>Delete Movie</t>
   </si>
   <si>
-    <t>Search Movie</t>
-  </si>
-  <si>
-    <t>Search Screen</t>
-  </si>
-  <si>
-    <t>Search Show</t>
-  </si>
-  <si>
-    <t>Show all Shows</t>
-  </si>
-  <si>
-    <t>Show all shows in a theatre</t>
-  </si>
-  <si>
     <t>Booking</t>
   </si>
   <si>
-    <t>choose seats</t>
-  </si>
-  <si>
-    <t>calculate total costs</t>
-  </si>
-  <si>
-    <t>choose payment method</t>
-  </si>
-  <si>
-    <t xml:space="preserve">make payment </t>
-  </si>
-  <si>
     <t>show ticket</t>
   </si>
   <si>
@@ -214,9 +187,6 @@
     <t>Seat</t>
   </si>
   <si>
-    <t>block seat</t>
-  </si>
-  <si>
     <t>book seat</t>
   </si>
   <si>
@@ -229,9 +199,6 @@
     <t>logout</t>
   </si>
   <si>
-    <t>Search screen</t>
-  </si>
-  <si>
     <t>2.3.1</t>
   </si>
   <si>
@@ -241,28 +208,10 @@
     <t>2.3.3</t>
   </si>
   <si>
-    <t>Add screen</t>
-  </si>
-  <si>
     <t>Add show</t>
   </si>
   <si>
     <t>Delete show</t>
-  </si>
-  <si>
-    <t>Search show</t>
-  </si>
-  <si>
-    <t>Show all shows</t>
-  </si>
-  <si>
-    <t>Show all shows in theatre</t>
-  </si>
-  <si>
-    <t>Choose seats</t>
-  </si>
-  <si>
-    <t>payment method $ make payment</t>
   </si>
   <si>
     <t>HTML page</t>
@@ -362,6 +311,54 @@
   </si>
   <si>
     <t>Cancel Seat</t>
+  </si>
+  <si>
+    <t>add Screen</t>
+  </si>
+  <si>
+    <t>delete Screen</t>
+  </si>
+  <si>
+    <t>Add Seat</t>
+  </si>
+  <si>
+    <t>Delete Seat</t>
+  </si>
+  <si>
+    <t>Update Screen</t>
+  </si>
+  <si>
+    <t>Add booking</t>
+  </si>
+  <si>
+    <t>delete booking</t>
+  </si>
+  <si>
+    <t>add ticket</t>
+  </si>
+  <si>
+    <t>Add movie</t>
+  </si>
+  <si>
+    <t>Delete movie</t>
+  </si>
+  <si>
+    <t>Search movie</t>
+  </si>
+  <si>
+    <t>view and update booking</t>
+  </si>
+  <si>
+    <t>add booking</t>
+  </si>
+  <si>
+    <t>view booking</t>
+  </si>
+  <si>
+    <t>update booking</t>
+  </si>
+  <si>
+    <t>add seat</t>
   </si>
 </sst>
 </file>
@@ -450,7 +447,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -469,12 +466,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -690,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1000"/>
+  <dimension ref="A1:C996"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -751,7 +752,7 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>49</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.4">
@@ -773,119 +774,100 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" customHeight="1">
-      <c r="C12" s="5" t="s">
+    <row r="12" spans="1:3" ht="14.4">
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" ht="15" hidden="1" customHeight="1"/>
+    <row r="14" spans="1:3" ht="14.4">
+      <c r="A14" s="1">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="14.4">
+      <c r="C15" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.4">
+      <c r="A17" s="1">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" customHeight="1">
+      <c r="C18" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" customHeight="1">
+      <c r="C19" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" customHeight="1">
+      <c r="C20" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" customHeight="1">
+      <c r="C21" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="14.4">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1" t="s">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="23" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="14.4">
-      <c r="C14" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="14.4">
-      <c r="A16" s="1">
-        <v>4</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="14.4">
-      <c r="C17" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="14.4">
-      <c r="C18" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="14.4">
-      <c r="A20" s="1">
-        <v>5</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C21" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C22" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1">
       <c r="C23" s="5" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1">
       <c r="C24" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1">
       <c r="C25" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="27" spans="1:3" ht="15.75" customHeight="1">
       <c r="A27">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1">
       <c r="C28" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C29" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="30" spans="1:3" ht="15.75" customHeight="1"/>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A31">
-        <v>7</v>
-      </c>
-      <c r="B31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1">
-      <c r="C32" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
+    <row r="31" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -1850,10 +1832,6 @@
     <row r="994" ht="15.75" customHeight="1"/>
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
-    <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -1864,8 +1842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -1915,10 +1893,10 @@
       <c r="A3" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="14"/>
+      <c r="C3" s="13"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -1949,7 +1927,7 @@
       <c r="D5" s="5">
         <v>1</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>44047</v>
       </c>
     </row>
@@ -1966,7 +1944,7 @@
       <c r="D6" s="5">
         <v>2</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <v>44047</v>
       </c>
     </row>
@@ -2004,7 +1982,7 @@
       <c r="D10" s="5">
         <v>1</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="14">
         <v>44047</v>
       </c>
     </row>
@@ -2021,7 +1999,7 @@
       <c r="D11" s="5">
         <v>1.5</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="14">
         <v>44047</v>
       </c>
     </row>
@@ -2041,7 +2019,7 @@
         <v>2.1</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -2073,7 +2051,7 @@
       <c r="D16" s="5">
         <v>1.5</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="14">
         <v>44053</v>
       </c>
     </row>
@@ -2090,7 +2068,7 @@
       <c r="D17" s="5">
         <v>1.5</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="14">
         <v>44053</v>
       </c>
     </row>
@@ -2099,7 +2077,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="14.4">
@@ -2128,7 +2106,7 @@
       <c r="D21" s="5">
         <v>1</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="14">
         <v>44053</v>
       </c>
     </row>
@@ -2145,7 +2123,7 @@
       <c r="D22" s="5">
         <v>1.5</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="14">
         <v>44053</v>
       </c>
     </row>
@@ -2155,12 +2133,12 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>10</v>
@@ -2173,7 +2151,7 @@
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1">
       <c r="A26" s="5" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>12</v>
@@ -2184,13 +2162,13 @@
       <c r="D26" s="5">
         <v>2</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26" s="14">
         <v>44053</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1">
       <c r="A27" s="5" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>28</v>
@@ -2201,7 +2179,7 @@
       <c r="D27" s="5">
         <v>1</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E27" s="14">
         <v>44053</v>
       </c>
     </row>
@@ -3199,7 +3177,7 @@
   <dimension ref="A1:F996"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -3249,10 +3227,10 @@
       <c r="A3" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" s="14"/>
+      <c r="B3" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="13"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -3280,8 +3258,12 @@
       <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="14">
+        <v>44047</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="14.4">
       <c r="A6" s="5" t="s">
@@ -3293,15 +3275,19 @@
       <c r="C6" s="5">
         <v>2</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="D6" s="5">
+        <v>2</v>
+      </c>
+      <c r="E6" s="14">
+        <v>44047</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="14.4">
       <c r="A8" s="5">
         <v>1.2</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="14.4">
@@ -3327,8 +3313,12 @@
       <c r="C10" s="5">
         <v>1</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="14">
+        <v>44047</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="14.4">
       <c r="A11" s="5" t="s">
@@ -3340,15 +3330,19 @@
       <c r="C11" s="5">
         <v>0.5</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="D11" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="14">
+        <v>44047</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="14.4">
       <c r="A13" s="5">
         <v>1.3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -3377,8 +3371,12 @@
       <c r="C15" s="5">
         <v>1</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="D15" s="5">
+        <v>1</v>
+      </c>
+      <c r="E15" s="14">
+        <v>44053</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="14.4">
       <c r="A16" s="5" t="s">
@@ -3390,8 +3388,12 @@
       <c r="C16" s="5">
         <v>3</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="D16" s="5">
+        <v>3</v>
+      </c>
+      <c r="E16" s="14">
+        <v>44053</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="14.4">
       <c r="A17" s="5"/>
@@ -3402,7 +3404,7 @@
         <v>1.4</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="14.4">
@@ -3428,8 +3430,12 @@
       <c r="C20" s="5">
         <v>1</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="12"/>
+      <c r="D20" s="5">
+        <v>1</v>
+      </c>
+      <c r="E20" s="15">
+        <v>44053</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="14.4">
       <c r="A21" s="5" t="s">
@@ -3441,8 +3447,12 @@
       <c r="C21" s="5">
         <v>1.5</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
+      <c r="D21" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="E21" s="16">
+        <v>44053</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1"/>
     <row r="23" spans="1:5" ht="15.75" customHeight="1">
@@ -3450,7 +3460,7 @@
         <v>1.5</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1">
@@ -3476,8 +3486,12 @@
       <c r="C25" s="5">
         <v>1</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="6"/>
+      <c r="D25" s="5">
+        <v>1</v>
+      </c>
+      <c r="E25" s="16">
+        <v>44053</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1">
       <c r="A26" s="5" t="s">
@@ -3489,8 +3503,12 @@
       <c r="C26" s="5">
         <v>1</v>
       </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
+      <c r="D26" s="5">
+        <v>1</v>
+      </c>
+      <c r="E26" s="14">
+        <v>44053</v>
+      </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1"/>
     <row r="28" spans="1:5" ht="15.75" customHeight="1"/>
@@ -4476,7 +4494,7 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -4515,7 +4533,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.4">
@@ -4523,7 +4541,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.4">
@@ -4549,8 +4567,12 @@
       <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="14">
+        <v>44047</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="14.4">
       <c r="A6" s="5" t="s">
@@ -4562,15 +4584,19 @@
       <c r="C6" s="5">
         <v>2</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="D6" s="5">
+        <v>2</v>
+      </c>
+      <c r="E6" s="14">
+        <v>44047</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="14.4">
       <c r="A8" s="5">
         <v>1.2</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="14.4">
@@ -4596,8 +4622,12 @@
       <c r="C10" s="5">
         <v>1.5</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="D10" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="E10" s="14">
+        <v>44047</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="14.4">
       <c r="A11" s="5" t="s">
@@ -4609,15 +4639,19 @@
       <c r="C11" s="5">
         <v>1.5</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="D11" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="E11" s="14">
+        <v>44047</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="14.4">
       <c r="A13" s="5">
         <v>1.3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.4">
@@ -4643,8 +4677,12 @@
       <c r="C15" s="5">
         <v>1.5</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="D15" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="E15" s="14">
+        <v>44053</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="14.4">
       <c r="A16" s="5" t="s">
@@ -4656,15 +4694,19 @@
       <c r="C16" s="5">
         <v>2</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="D16" s="5">
+        <v>2</v>
+      </c>
+      <c r="E16" s="14">
+        <v>44053</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="14.4">
       <c r="A18" s="5">
         <v>1.4</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="14.4">
@@ -4690,8 +4732,12 @@
       <c r="C20" s="5">
         <v>1</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
+      <c r="D20" s="5">
+        <v>1</v>
+      </c>
+      <c r="E20" s="14">
+        <v>44053</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1">
       <c r="A21" s="5" t="s">
@@ -4703,8 +4749,12 @@
       <c r="C21" s="5">
         <v>2</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="D21" s="5">
+        <v>2</v>
+      </c>
+      <c r="E21" s="14">
+        <v>44053</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1"/>
     <row r="23" spans="1:5" ht="15.75" customHeight="1">
@@ -4712,7 +4762,7 @@
         <v>1.5</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1">
@@ -4720,7 +4770,7 @@
         <v>25</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="C24" s="5">
         <v>1</v>
@@ -4736,6 +4786,12 @@
       <c r="C25" s="5">
         <v>1</v>
       </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" s="17">
+        <v>44053</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1">
       <c r="A26" t="s">
@@ -4746,6 +4802,12 @@
       </c>
       <c r="C26" s="5">
         <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" s="17">
+        <v>44053</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1"/>
@@ -5732,8 +5794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{153E3325-7D88-448F-881D-269201243192}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -5759,7 +5821,7 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F1" t="s">
         <v>7</v>
@@ -5778,7 +5840,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.4">
@@ -5786,7 +5848,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="C4" s="11">
         <v>3</v>
@@ -5802,6 +5864,12 @@
       <c r="C5" s="11">
         <v>1</v>
       </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="17">
+        <v>44047</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="14.4">
       <c r="A6" s="10" t="s">
@@ -5813,13 +5881,19 @@
       <c r="C6" s="11">
         <v>1.5</v>
       </c>
+      <c r="D6">
+        <v>1.5</v>
+      </c>
+      <c r="E6" s="17">
+        <v>44047</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="14.4">
       <c r="A8">
         <v>1.2</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>47</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="14.4">
@@ -5827,7 +5901,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="C9" s="11">
         <v>2</v>
@@ -5843,6 +5917,12 @@
       <c r="C10" s="11">
         <v>1.5</v>
       </c>
+      <c r="D10">
+        <v>1.5</v>
+      </c>
+      <c r="E10" s="17">
+        <v>44047</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="14.4">
       <c r="A11" s="10" t="s">
@@ -5854,13 +5934,19 @@
       <c r="C11" s="11">
         <v>1.5</v>
       </c>
+      <c r="D11">
+        <v>1.5</v>
+      </c>
+      <c r="E11" s="17">
+        <v>44047</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="14.4">
       <c r="A13">
         <v>1.3</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.4">
@@ -5884,37 +5970,49 @@
       <c r="C15" s="11">
         <v>1.5</v>
       </c>
+      <c r="D15">
+        <v>1.5</v>
+      </c>
+      <c r="E15" s="17">
+        <v>44053</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="14.4">
       <c r="A16" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C16" s="11">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="14.4">
+      <c r="D16">
+        <v>1.5</v>
+      </c>
+      <c r="E16" s="17">
+        <v>44053</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="14.4">
       <c r="A18">
         <v>2</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="14.4">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.4">
       <c r="A19">
         <v>2.1</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="14.4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.4">
       <c r="A20" s="8" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>34</v>
@@ -5923,7 +6021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.4">
+    <row r="21" spans="1:5" ht="14.4">
       <c r="A21" s="10" t="s">
         <v>29</v>
       </c>
@@ -5933,27 +6031,39 @@
       <c r="C21" s="11">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="14.4">
+      <c r="D21">
+        <v>2.5</v>
+      </c>
+      <c r="E21" s="17">
+        <v>44053</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="14.4">
       <c r="A22" s="10" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C22" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="14.4">
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="17">
+        <v>44053</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="14.4">
       <c r="A24">
         <v>2.2000000000000002</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="14.4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="14.4">
       <c r="A25" s="10" t="s">
         <v>31</v>
       </c>
@@ -5964,7 +6074,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14.4">
+    <row r="26" spans="1:5" ht="14.4">
       <c r="A26" s="10" t="s">
         <v>32</v>
       </c>
@@ -5974,30 +6084,42 @@
       <c r="C26" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="14.4">
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" s="17">
+        <v>44053</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="14.4">
       <c r="A27" s="10" t="s">
         <v>33</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C27" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="14.4">
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27" s="17">
+        <v>44053</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="14.4">
       <c r="A29">
         <v>2.2999999999999998</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="C29" s="11"/>
     </row>
-    <row r="30" spans="1:3" ht="14.4">
+    <row r="30" spans="1:5" ht="14.4">
       <c r="A30" s="10" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>34</v>
@@ -6006,9 +6128,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.4">
+    <row r="31" spans="1:5" ht="14.4">
       <c r="A31" s="10" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>12</v>
@@ -6017,12 +6139,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.4">
+    <row r="32" spans="1:5" ht="14.4">
       <c r="A32" s="10" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C32" s="11">
         <v>2</v>

</xml_diff>